<commit_message>
National 2 files added
</commit_message>
<xml_diff>
--- a/code/data/candidate_counts.xlsx
+++ b/code/data/candidate_counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fc2bdd364c40744/Documents/STA/Dresscode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1282" documentId="8_{12DB0E01-272D-3345-9D4A-E9BABBACF14F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{13AE0DC0-FF90-435E-9166-08396A9B8F9E}"/>
+  <xr:revisionPtr revIDLastSave="1363" documentId="8_{12DB0E01-272D-3345-9D4A-E9BABBACF14F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D1F7CE4A-8DF4-4D9A-99B2-46E2FD5E27F8}"/>
   <bookViews>
-    <workbookView xWindow="10476" yWindow="216" windowWidth="12492" windowHeight="11652" firstSheet="1" activeTab="2" xr2:uid="{561839FE-D5DF-5443-A07F-CBA9FC630A07}"/>
+    <workbookView xWindow="10932" yWindow="900" windowWidth="11820" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{561839FE-D5DF-5443-A07F-CBA9FC630A07}"/>
   </bookViews>
   <sheets>
     <sheet name="total_candidates" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="95">
   <si>
     <t>all-National2</t>
   </si>
@@ -753,10 +753,10 @@
   <dimension ref="A1:CH37"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BY17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BU20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BY33" sqref="BY33:CC36"/>
+      <selection pane="bottomRight" activeCell="BY36" sqref="BY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1920,6 +1920,12 @@
       <c r="BV31" s="2">
         <v>260</v>
       </c>
+      <c r="BW31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX31" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY31" s="1">
         <v>12241</v>
       </c>
@@ -2010,6 +2016,21 @@
         <v>78</v>
       </c>
       <c r="BS32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT32" s="1">
+        <v>1072</v>
+      </c>
+      <c r="BU32" s="1">
+        <v>675</v>
+      </c>
+      <c r="BV32" s="1">
+        <v>397</v>
+      </c>
+      <c r="BW32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY32" s="1">
@@ -2094,6 +2115,21 @@
       <c r="BS33" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT33" s="1">
+        <v>1297</v>
+      </c>
+      <c r="BU33" s="1">
+        <v>832</v>
+      </c>
+      <c r="BV33" s="1">
+        <v>465</v>
+      </c>
+      <c r="BW33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX33" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY33" s="1" t="s">
         <v>78</v>
       </c>
@@ -2166,6 +2202,21 @@
       <c r="BS34" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT34" s="1">
+        <v>1122</v>
+      </c>
+      <c r="BU34" s="1">
+        <v>703</v>
+      </c>
+      <c r="BV34" s="1">
+        <v>419</v>
+      </c>
+      <c r="BW34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX34" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY34" s="1" t="s">
         <v>78</v>
       </c>
@@ -2236,6 +2287,21 @@
       <c r="BS35" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT35" s="1">
+        <v>1213</v>
+      </c>
+      <c r="BU35" s="1">
+        <v>783</v>
+      </c>
+      <c r="BV35" s="1">
+        <v>430</v>
+      </c>
+      <c r="BW35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX35" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY35" s="1" t="s">
         <v>78</v>
       </c>
@@ -2314,6 +2380,21 @@
         <v>1</v>
       </c>
       <c r="BS36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT36" s="1">
+        <v>1202</v>
+      </c>
+      <c r="BU36" s="1">
+        <v>802</v>
+      </c>
+      <c r="BV36" s="1">
+        <v>400</v>
+      </c>
+      <c r="BW36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY36" s="1" t="s">
@@ -2347,10 +2428,10 @@
   <dimension ref="A1:CH37"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BY17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BU21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CD32" sqref="CD32"/>
+      <selection pane="bottomRight" activeCell="BY36" sqref="BY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3658,6 +3739,12 @@
       <c r="BV31" s="2">
         <v>388</v>
       </c>
+      <c r="BW31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX31" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY31" s="1">
         <v>18679</v>
       </c>
@@ -3748,6 +3835,21 @@
         <v>78</v>
       </c>
       <c r="BS32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT32" s="1">
+        <v>1933</v>
+      </c>
+      <c r="BU32" s="1">
+        <v>1212</v>
+      </c>
+      <c r="BV32" s="1">
+        <v>721</v>
+      </c>
+      <c r="BW32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY32" s="1">
@@ -3832,6 +3934,21 @@
       <c r="BS33" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT33" s="1">
+        <v>2465</v>
+      </c>
+      <c r="BU33" s="1">
+        <v>1581</v>
+      </c>
+      <c r="BV33" s="1">
+        <v>884</v>
+      </c>
+      <c r="BW33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX33" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY33" s="1" t="s">
         <v>78</v>
       </c>
@@ -3904,6 +4021,21 @@
       <c r="BS34" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT34" s="1">
+        <v>1915</v>
+      </c>
+      <c r="BU34" s="1">
+        <v>1190</v>
+      </c>
+      <c r="BV34" s="1">
+        <v>725</v>
+      </c>
+      <c r="BW34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX34" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY34" s="1" t="s">
         <v>78</v>
       </c>
@@ -3974,6 +4106,21 @@
       <c r="BS35" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT35" s="1">
+        <v>2105</v>
+      </c>
+      <c r="BU35" s="1">
+        <v>1348</v>
+      </c>
+      <c r="BV35" s="1">
+        <v>757</v>
+      </c>
+      <c r="BW35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX35" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY35" s="1" t="s">
         <v>78</v>
       </c>
@@ -4052,6 +4199,21 @@
         <v>1</v>
       </c>
       <c r="BS36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT36" s="1">
+        <v>2044</v>
+      </c>
+      <c r="BU36" s="1">
+        <v>1359</v>
+      </c>
+      <c r="BV36" s="1">
+        <v>685</v>
+      </c>
+      <c r="BW36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY36" s="1" t="s">
@@ -4085,10 +4247,10 @@
   <dimension ref="A1:CH37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="BY17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="BU20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CD32" sqref="CD32"/>
+      <selection pane="bottomRight" activeCell="BY36" sqref="BY36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -5390,6 +5552,12 @@
       <c r="BV31" s="2">
         <v>308</v>
       </c>
+      <c r="BW31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX31" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY31" s="1">
         <v>13738</v>
       </c>
@@ -5480,6 +5648,21 @@
         <v>78</v>
       </c>
       <c r="BS32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT32" s="1">
+        <v>1545</v>
+      </c>
+      <c r="BU32" s="1">
+        <v>966</v>
+      </c>
+      <c r="BV32" s="1">
+        <v>579</v>
+      </c>
+      <c r="BW32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX32" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY32" s="1">
@@ -5564,6 +5747,21 @@
       <c r="BS33" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT33" s="1">
+        <v>1923</v>
+      </c>
+      <c r="BU33" s="1">
+        <v>1216</v>
+      </c>
+      <c r="BV33" s="1">
+        <v>707</v>
+      </c>
+      <c r="BW33" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX33" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY33" s="1" t="s">
         <v>78</v>
       </c>
@@ -5636,6 +5834,21 @@
       <c r="BS34" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT34" s="1">
+        <v>1594</v>
+      </c>
+      <c r="BU34" s="1">
+        <v>991</v>
+      </c>
+      <c r="BV34" s="1">
+        <v>603</v>
+      </c>
+      <c r="BW34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX34" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY34" s="1" t="s">
         <v>78</v>
       </c>
@@ -5706,6 +5919,21 @@
       <c r="BS35" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="BT35" s="1">
+        <v>1740</v>
+      </c>
+      <c r="BU35" s="1">
+        <v>1109</v>
+      </c>
+      <c r="BV35" s="1">
+        <v>631</v>
+      </c>
+      <c r="BW35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX35" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="BY35" s="1" t="s">
         <v>78</v>
       </c>
@@ -5784,6 +6012,21 @@
         <v>1</v>
       </c>
       <c r="BS36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BT36" s="1">
+        <v>1629</v>
+      </c>
+      <c r="BU36" s="1">
+        <v>1079</v>
+      </c>
+      <c r="BV36" s="1">
+        <v>550</v>
+      </c>
+      <c r="BW36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="BX36" s="1" t="s">
         <v>78</v>
       </c>
       <c r="BY36" s="1" t="s">

</xml_diff>